<commit_message>
Organized pDC DEG analyis
Reran with PtRem label and improved gene expression analysis of pDCs.
</commit_message>
<xml_diff>
--- a/4_XV-seq/XV-seq_overview.xlsx
+++ b/4_XV-seq/XV-seq_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vangalen/Dropbox (Partners HealthCare)/Projects/Single-cell_BPDCN/AnalysisPeter/Github/4_XV-seq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5225BDF9-71BB-AE42-B368-E6ED3B87F024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C648CEA0-8A0A-0C4A-8FE1-6C0BEE33FF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XV-seq_overview" sheetId="1" r:id="rId1"/>
@@ -211,9 +211,6 @@
     <t>Pt12Rel</t>
   </si>
   <si>
-    <t>Pt1Mrd</t>
-  </si>
-  <si>
     <t>Pt10Dx/RPS24.40/Patient10_RPS24.40_summTable.txt</t>
   </si>
   <si>
@@ -223,21 +220,6 @@
     <t>Pt10Dx/SMARCD1.1330/Patient10_SMARCD1.1330_summTable.txt</t>
   </si>
   <si>
-    <t>Pt1Mrd/FAM98C.903/Patient1MRD_FAM98C.903_summTable.txt</t>
-  </si>
-  <si>
-    <t>Pt1Mrd/SETX.10691/Patient1MRD_SETX.10691_summTable.txt</t>
-  </si>
-  <si>
-    <t>Pt1Mrd/ASXL1.2046/Patient1MRD_ASXL1.2046_summTable.txt</t>
-  </si>
-  <si>
-    <t>Pt1Mrd/TET2.2847/Patient1MRD_TET2.2847_summTable.txt</t>
-  </si>
-  <si>
-    <t>Pt1Mrd/SMARCC1.5233/Patient1MRD_SMARCC1.5233_summTable.txt</t>
-  </si>
-  <si>
     <t>Pt5Dx/TET2.796/Patient5_TET2.796_summTable.txt</t>
   </si>
   <si>
@@ -746,6 +728,24 @@
   </si>
   <si>
     <t>BM involvement</t>
+  </si>
+  <si>
+    <t>Pt1Rem</t>
+  </si>
+  <si>
+    <t>Pt1Rem/TET2.2847/Patient1Rem_TET2.2847_summTable.txt</t>
+  </si>
+  <si>
+    <t>Pt1Rem/ASXL1.2046/Patient1Rem_ASXL1.2046_summTable.txt</t>
+  </si>
+  <si>
+    <t>Pt1Rem/SMARCC1.5233/Patient1Rem_SMARCC1.5233_summTable.txt</t>
+  </si>
+  <si>
+    <t>Pt1Rem/FAM98C.903/Patient1Rem_FAM98C.903_summTable.txt</t>
+  </si>
+  <si>
+    <t>Pt1Rem/SETX.10691/Patient1Rem_SETX.10691_summTable.txt</t>
   </si>
 </sst>
 </file>
@@ -1748,9 +1748,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1775,34 +1775,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C1" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>233</v>
-      </c>
-      <c r="E1" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="G1" s="35" t="s">
-        <v>146</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="K1" s="24" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>1</v>
@@ -1813,35 +1813,35 @@
         <v>35</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E2" s="4">
         <v>1.01091791346542</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="K2" s="25">
         <v>6415</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
@@ -1849,35 +1849,35 @@
         <v>35</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E3" s="4">
         <v>0.242620299231702</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="K3" s="25">
         <v>2555</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
@@ -1885,37 +1885,37 @@
         <v>35</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E4" s="4">
         <v>2.9518803073190401</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J4" s="21" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="K4" s="25">
         <v>225</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
@@ -1923,37 +1923,37 @@
         <v>35</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E5" s="4">
         <v>6.0250707642539396</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="J5" s="22" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="K5" s="26">
         <v>324</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.15">
@@ -1961,223 +1961,223 @@
         <v>35</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E6" s="9">
         <v>4.5693489688637197</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="K6" s="27">
         <v>120</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>59</v>
+        <v>232</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E7" s="4">
         <v>1.0861132660977499</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="12" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K7" s="28" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>66</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>59</v>
+        <v>232</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E8" s="4">
         <v>0.28122575640031</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K8" s="29" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>65</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>59</v>
+        <v>232</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E9" s="4">
         <v>2.4825446082234199</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K9" s="29" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>67</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>59</v>
+        <v>232</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E10" s="4">
         <v>6.5554693560899899</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K10" s="29" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>63</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11" s="8" t="s">
-        <v>59</v>
+        <v>232</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E11" s="9">
         <v>4.4511249030256002</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K11" s="30" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>64</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
@@ -2185,35 +2185,35 @@
         <v>56</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E12" s="4">
         <v>4.2702050663449898</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="20" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="J12" s="20" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="K12" s="25">
         <v>8449</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
@@ -2221,35 +2221,35 @@
         <v>56</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E13" s="4">
         <v>5.4764776839565696</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="20" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="K13" s="25">
         <v>5109</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.15">
@@ -2257,35 +2257,35 @@
         <v>56</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E14" s="9">
         <v>5.9831121833534304</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="15" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="K14" s="27">
         <v>942</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
@@ -2293,31 +2293,31 @@
         <v>36</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E15" s="4">
         <v>9.8609904430929607</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="K15" s="31">
         <v>5002</v>
@@ -2331,31 +2331,31 @@
         <v>36</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E16" s="4">
         <v>3.8444830582102498</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K16" s="26">
         <v>4701</v>
@@ -2369,31 +2369,31 @@
         <v>36</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E17" s="9">
         <v>1.62901824500434</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H17" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="J17" s="15" t="s">
         <v>150</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="J17" s="15" t="s">
-        <v>156</v>
       </c>
       <c r="K17" s="27">
         <v>11002</v>
@@ -2407,31 +2407,31 @@
         <v>37</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E18" s="11">
         <v>1.22699386503067</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="K18" s="29">
         <v>6953</v>
@@ -2445,31 +2445,31 @@
         <v>37</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E19" s="11">
         <v>1.0686720759944499</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="K19" s="29">
         <v>6215</v>
@@ -2483,31 +2483,31 @@
         <v>37</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E20" s="11">
         <v>1.1379378586978</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="K20" s="29">
         <v>5667</v>
@@ -2521,31 +2521,31 @@
         <v>37</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E21" s="11">
         <v>1.88007124480506</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="K21" s="29">
         <v>5189</v>
@@ -2559,31 +2559,31 @@
         <v>37</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E22" s="11">
         <v>27.646942410449199</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="K22" s="32">
         <v>6681</v>
@@ -2597,28 +2597,28 @@
         <v>37</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E23" s="11">
         <v>0.41559469622006701</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="K23" s="32">
         <v>2760</v>
@@ -2632,31 +2632,31 @@
         <v>37</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E24" s="11">
         <v>9.8357411438749196</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>10</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="K24" s="32">
         <v>2622</v>
@@ -2670,31 +2670,31 @@
         <v>37</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E25" s="11">
         <v>0.24737779536908699</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>10</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="K25" s="32">
         <v>1515</v>
@@ -2708,31 +2708,31 @@
         <v>37</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E26" s="11">
         <v>6.1844448842271902</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="K26" s="32">
         <v>1454</v>
@@ -2746,31 +2746,31 @@
         <v>37</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E27" s="11">
         <v>1.20720364140114</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="K27" s="32">
         <v>2090</v>
@@ -2784,31 +2784,31 @@
         <v>37</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E28" s="11">
         <v>13.2000791608945</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="K28" s="32">
         <v>1816</v>
@@ -2902,37 +2902,37 @@
         <v>37</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E33" s="4">
         <v>35.751038986740497</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="K33" s="29">
         <v>350</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:12" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -2940,37 +2940,37 @@
         <v>37</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E34" s="4">
         <v>98.990698594894099</v>
       </c>
       <c r="F34" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G34" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="G34" s="11" t="s">
-        <v>137</v>
-      </c>
       <c r="H34" s="7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="K34" s="7">
         <v>421</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.15">
@@ -2978,37 +2978,37 @@
         <v>37</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E35" s="4">
         <v>4.8288145656045902</v>
       </c>
       <c r="F35" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G35" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="H35" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="H35" s="7" t="s">
-        <v>143</v>
-      </c>
       <c r="I35" s="7" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="K35" s="7">
         <v>3296</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.15">
@@ -3016,37 +3016,37 @@
         <v>37</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E36" s="9">
         <v>0.77181872155155296</v>
       </c>
       <c r="F36" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G36" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="G36" s="9" t="s">
-        <v>137</v>
-      </c>
       <c r="H36" s="10" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="K36" s="10">
         <v>1824</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.15">
@@ -3054,34 +3054,34 @@
         <v>23</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E37" s="4">
         <v>2.6940517471325598</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K37" s="29" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L37" s="3" t="s">
         <v>31</v>
@@ -3092,34 +3092,34 @@
         <v>23</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E38" s="4">
         <v>3.3208855694851902</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K38" s="29" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>32</v>
@@ -3130,34 +3130,34 @@
         <v>23</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E39" s="4">
         <v>3.0808215524139699</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K39" s="29" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>33</v>
@@ -3168,34 +3168,34 @@
         <v>23</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E40" s="4">
         <v>5.1347025873566201</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K40" s="29" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L40" s="3" t="s">
         <v>34</v>
@@ -3206,34 +3206,34 @@
         <v>23</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E41" s="4">
         <v>29.6345692184582</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K41" s="29" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L41" s="3" t="s">
         <v>24</v>
@@ -3244,32 +3244,32 @@
         <v>23</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E42" s="4">
         <v>0.89357161909842597</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H42" s="3"/>
       <c r="I42" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K42" s="29" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L42" s="3" t="s">
         <v>25</v>
@@ -3280,34 +3280,34 @@
         <v>23</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E43" s="4">
         <v>10.282742064550501</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K43" s="29" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L43" s="3" t="s">
         <v>26</v>
@@ -3318,34 +3318,34 @@
         <v>23</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E44" s="4">
         <v>0.25340090690850797</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K44" s="29" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L44" s="3" t="s">
         <v>27</v>
@@ -3356,34 +3356,34 @@
         <v>23</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E45" s="4">
         <v>20.085356094958598</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K45" s="29" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L45" s="3" t="s">
         <v>28</v>
@@ -3394,34 +3394,34 @@
         <v>23</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E46" s="4">
         <v>2.8007468658308801</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K46" s="29" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L46" s="3" t="s">
         <v>29</v>
@@ -3432,37 +3432,37 @@
         <v>23</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E47" s="4">
         <v>28.540944251800401</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K47" s="29" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.15">
@@ -3482,7 +3482,7 @@
       <c r="J48" s="18"/>
       <c r="K48" s="34"/>
       <c r="L48" s="18" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.15">
@@ -3502,7 +3502,7 @@
       <c r="J49" s="18"/>
       <c r="K49" s="34"/>
       <c r="L49" s="18" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.15">
@@ -3522,7 +3522,7 @@
       <c r="J50" s="18"/>
       <c r="K50" s="34"/>
       <c r="L50" s="18" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.15">
@@ -3542,7 +3542,7 @@
       <c r="J51" s="18"/>
       <c r="K51" s="34"/>
       <c r="L51" s="18" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.15">
@@ -3550,34 +3550,34 @@
         <v>23</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E52" s="9">
         <v>37.623366230994897</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J52" s="8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K52" s="30" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L52" s="8" t="s">
         <v>30</v>
@@ -3588,35 +3588,35 @@
         <v>57</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E53" s="4">
         <v>0.39347129116875501</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H53" s="6"/>
       <c r="I53" s="6" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="K53" s="6">
         <v>4684</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.15">
@@ -3624,37 +3624,37 @@
         <v>57</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E54" s="4">
         <v>8.7438064704167803E-2</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="K54" s="6" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.15">
@@ -3662,37 +3662,37 @@
         <v>57</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E55" s="4">
         <v>1.50102011075488</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="K55" s="6">
         <v>527</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.15">
@@ -3700,37 +3700,37 @@
         <v>57</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E56" s="9">
         <v>2.7980180705333701</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="I56" s="10" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="K56" s="10">
         <v>2572</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.15">
@@ -3738,35 +3738,35 @@
         <v>58</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E57" s="4">
         <v>22.822201317027201</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H57" s="3"/>
       <c r="I57" s="12" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J57" s="12" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K57" s="28" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.15">
@@ -3774,37 +3774,37 @@
         <v>58</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E58" s="4">
         <v>11.0253998118532</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K58" s="29" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.15">
@@ -3812,37 +3812,37 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E59" s="4">
         <v>8.5042333019755407</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K59" s="29" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L59" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.15">
@@ -3850,397 +3850,397 @@
         <v>58</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E60" s="9">
         <v>8.4101599247412899</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="J60" s="8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K60" s="30" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="L60" s="8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A61" s="5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E61" s="11">
         <v>5.9118644067796602</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H61" s="3"/>
       <c r="I61" s="5" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="J61" s="32" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="K61" s="5">
         <v>870</v>
       </c>
       <c r="L61" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A62" s="5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E62" s="4">
         <v>9.6406779661016895</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H62" s="3"/>
       <c r="I62" s="5" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="J62" s="32" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="K62" s="5">
         <v>2158</v>
       </c>
       <c r="L62" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A63" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E63" s="9">
         <v>40.786440677966098</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H63" s="8"/>
       <c r="I63" s="8" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="J63" s="30" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="K63" s="8">
         <v>1234</v>
       </c>
       <c r="L63" s="8" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A64" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E64" s="11">
         <v>1.44092219020172</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H64" s="3"/>
       <c r="I64" s="32" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="J64" s="32" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K64" s="5">
         <v>2249</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A65" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E65" s="11">
         <v>4.5533141210374604</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H65" s="3"/>
       <c r="I65" s="32" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="J65" s="32" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="K65" s="5">
         <v>4785</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A66" s="8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E66" s="9">
         <v>83.775216138328503</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H66" s="8"/>
       <c r="I66" s="30" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="J66" s="30" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="K66" s="8">
         <v>805</v>
       </c>
       <c r="L66" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A67" s="5" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E67" s="11">
         <v>1.57232704402515</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H67" s="3"/>
       <c r="I67" s="5" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="J67" s="32" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="K67" s="5">
         <v>2601</v>
       </c>
       <c r="L67" s="5" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A68" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E68" s="4">
         <v>5.3009883198562404</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H68" s="3"/>
       <c r="I68" s="5" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="J68" s="32" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="K68" s="5">
         <v>6953</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A69" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E69" s="4">
         <v>4.8966756513926297</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H69" s="3"/>
       <c r="I69" s="3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="J69" s="29" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="K69" s="3">
         <v>6699</v>
       </c>
       <c r="L69" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A70" s="8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E70" s="9">
         <v>0.494159928122192</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H70" s="8"/>
       <c r="I70" s="8" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="J70" s="30" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="K70" s="8">
         <v>1137</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>